<commit_message>
lister les lieux sans le mobile first
</commit_message>
<xml_diff>
--- a/Maquette et autre/LIEUX ASSOCIATION.xlsx
+++ b/Maquette et autre/LIEUX ASSOCIATION.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frede\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2119EC-3AA0-414D-AD1F-08ABAF3E98CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="910" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1 - COORDONNEES" sheetId="6" r:id="rId1"/>
@@ -22,7 +16,7 @@
     <sheet name="7 - LAVE LINGE" sheetId="8" r:id="rId7"/>
     <sheet name="SERVICES AUTRES" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -494,7 +488,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-40C]General"/>
   </numFmts>
@@ -1541,6 +1535,24 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1562,24 +1574,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1596,6 +1590,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1610,55 +1628,31 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="6" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1670,7 +1664,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1735,7 +1729,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1770,7 +1764,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1947,21 +1941,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1975,41 +1969,41 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
     </row>
     <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="F4" s="23">
         <f ca="1">TODAY()</f>
-        <v>43802</v>
+        <v>43843</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="3" t="s">
         <v>47</v>
       </c>
@@ -2021,11 +2015,11 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="5" t="s">
         <v>120</v>
       </c>
@@ -2037,12 +2031,12 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="85"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="87"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="77"/>
     </row>
     <row r="9" spans="1:6" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="88" t="s">
@@ -2059,12 +2053,12 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="85"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="87"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="77"/>
     </row>
     <row r="11" spans="1:6" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="91" t="s">
@@ -2083,19 +2077,19 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="85"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="87"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
     </row>
     <row r="13" spans="1:6" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="84"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="66" t="s">
         <v>109</v>
       </c>
@@ -2105,19 +2099,19 @@
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="85"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="87"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="77"/>
     </row>
     <row r="15" spans="1:6" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="83"/>
-      <c r="C15" s="84"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="80"/>
       <c r="D15" s="5" t="s">
         <v>54</v>
       </c>
@@ -2129,19 +2123,19 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="85"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="87"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="77"/>
     </row>
     <row r="17" spans="1:6" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="82" t="s">
+      <c r="A17" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="83"/>
-      <c r="C17" s="84"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="80"/>
       <c r="D17" s="5" t="s">
         <v>56</v>
       </c>
@@ -2151,19 +2145,19 @@
       <c r="F17" s="21"/>
     </row>
     <row r="18" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="85"/>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="87"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="77"/>
     </row>
     <row r="19" spans="1:6" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="83"/>
-      <c r="C19" s="84"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="80"/>
       <c r="D19" s="5" t="s">
         <v>58</v>
       </c>
@@ -2173,20 +2167,15 @@
       <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="85"/>
-      <c r="B20" s="86"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="87"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:F20"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A6:C6"/>
@@ -2199,6 +2188,11 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="85" orientation="landscape" verticalDpi="300" r:id="rId1"/>
@@ -2206,14 +2200,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2225,53 +2219,53 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
     </row>
     <row r="4" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="L4" s="18">
         <f ca="1">TODAY()</f>
-        <v>43802</v>
+        <v>43843</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
@@ -2301,18 +2295,18 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="94" t="s">
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="101"/>
+      <c r="F7" s="106"/>
       <c r="G7" s="14" t="s">
         <v>8</v>
       </c>
@@ -2325,16 +2319,16 @@
       <c r="J7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="96"/>
     </row>
     <row r="8" spans="1:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="80"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="102"/>
+      <c r="A8" s="86"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="107"/>
       <c r="G8" s="9" t="s">
         <v>10</v>
       </c>
@@ -2345,33 +2339,33 @@
       <c r="J8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="100"/>
-      <c r="L8" s="100"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
     </row>
     <row r="9" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="85"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="87"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="77"/>
     </row>
     <row r="10" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="94" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="94" t="s">
+      <c r="E10" s="102" t="s">
         <v>68</v>
       </c>
       <c r="F10" s="15"/>
@@ -2379,15 +2373,15 @@
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
-      <c r="K10" s="100"/>
-      <c r="L10" s="100"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="96"/>
     </row>
     <row r="11" spans="1:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="105"/>
-      <c r="B11" s="106"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
       <c r="F11" s="11" t="s">
         <v>12</v>
       </c>
@@ -2403,33 +2397,33 @@
       <c r="J11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="100"/>
-      <c r="L11" s="100"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="96"/>
     </row>
     <row r="12" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="85"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="87"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="77"/>
     </row>
     <row r="13" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="94" t="s">
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="94" t="s">
+      <c r="E13" s="102" t="s">
         <v>34</v>
       </c>
       <c r="F13" s="14" t="s">
@@ -2450,62 +2444,62 @@
       <c r="K13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="100"/>
+      <c r="L13" s="96"/>
     </row>
     <row r="14" spans="1:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="105"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="95"/>
+      <c r="A14" s="99"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="100"/>
+      <c r="L14" s="96"/>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="85"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
-      <c r="L15" s="87"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="77"/>
     </row>
     <row r="16" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="83"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="94" t="s">
+      <c r="B16" s="79"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="94" t="s">
+      <c r="E16" s="102" t="s">
         <v>68</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="96"/>
-      <c r="K16" s="98"/>
-      <c r="L16" s="98"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="97"/>
     </row>
     <row r="17" spans="1:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="105"/>
-      <c r="B17" s="106"/>
-      <c r="C17" s="107"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="103"/>
       <c r="F17" s="13" t="s">
         <v>10</v>
       </c>
@@ -2518,35 +2512,48 @@
       <c r="I17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J17" s="97"/>
-      <c r="K17" s="99"/>
-      <c r="L17" s="99"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="98"/>
     </row>
     <row r="18" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="85"/>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
-      <c r="L18" s="87"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
+      <c r="L18" s="77"/>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="103" t="s">
+      <c r="B20" s="94" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="104"/>
+      <c r="B21" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="K10:K11"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A3:L3"/>
@@ -2563,19 +2570,6 @@
     <mergeCell ref="A10:C11"/>
     <mergeCell ref="A13:C14"/>
     <mergeCell ref="A16:C17"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="K10:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="85" orientation="landscape" verticalDpi="300" r:id="rId1"/>
@@ -2583,7 +2577,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2607,55 +2601,55 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
     </row>
     <row r="4" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="M4" s="18">
         <f ca="1">TODAY()</f>
-        <v>43802</v>
+        <v>43843</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:13" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
@@ -2688,21 +2682,21 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="94" t="s">
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="94" t="s">
+      <c r="F7" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="G7" s="101"/>
+      <c r="G7" s="106"/>
       <c r="H7" s="14" t="s">
         <v>8</v>
       </c>
@@ -2718,16 +2712,16 @@
       <c r="L7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="100"/>
+      <c r="M7" s="96"/>
     </row>
     <row r="8" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="80"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="102"/>
+      <c r="A8" s="86"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="107"/>
       <c r="H8" s="9" t="s">
         <v>10</v>
       </c>
@@ -2737,36 +2731,36 @@
       <c r="J8" s="74"/>
       <c r="K8" s="10"/>
       <c r="L8" s="74"/>
-      <c r="M8" s="100"/>
+      <c r="M8" s="96"/>
     </row>
     <row r="9" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="85"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="87"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="77"/>
     </row>
     <row r="10" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="94" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="102" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="94" t="s">
+      <c r="F10" s="102" t="s">
         <v>119</v>
       </c>
       <c r="G10" s="15"/>
@@ -2774,18 +2768,18 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
-      <c r="L10" s="100"/>
-      <c r="M10" s="100"/>
+      <c r="L10" s="96"/>
+      <c r="M10" s="96"/>
     </row>
     <row r="11" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="105"/>
-      <c r="B11" s="106"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="95"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="103"/>
       <c r="E11" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="95"/>
+      <c r="F11" s="103"/>
       <c r="G11" s="11" t="s">
         <v>100</v>
       </c>
@@ -2801,37 +2795,37 @@
       <c r="K11" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="L11" s="100"/>
-      <c r="M11" s="100"/>
+      <c r="L11" s="96"/>
+      <c r="M11" s="96"/>
     </row>
     <row r="12" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="85"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="87"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="77"/>
     </row>
     <row r="13" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="94" t="s">
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="102" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="108" t="s">
         <v>117</v>
       </c>
-      <c r="F13" s="94" t="s">
+      <c r="F13" s="102" t="s">
         <v>119</v>
       </c>
       <c r="G13" s="14" t="s">
@@ -2840,80 +2834,80 @@
       <c r="H13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="100"/>
+      <c r="I13" s="96"/>
       <c r="J13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="100"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="100"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="96"/>
+      <c r="M13" s="96"/>
     </row>
     <row r="14" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="105"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="95"/>
+      <c r="A14" s="99"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="103"/>
       <c r="E14" s="109"/>
-      <c r="F14" s="95"/>
+      <c r="F14" s="103"/>
       <c r="G14" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="100"/>
+      <c r="I14" s="96"/>
       <c r="J14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="100"/>
-      <c r="L14" s="100"/>
-      <c r="M14" s="100"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="96"/>
+      <c r="M14" s="96"/>
     </row>
     <row r="15" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="85"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
-      <c r="L15" s="86"/>
-      <c r="M15" s="87"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="77"/>
     </row>
     <row r="16" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="83"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="94" t="s">
+      <c r="B16" s="79"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="94" t="s">
+      <c r="E16" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="94" t="s">
+      <c r="F16" s="102" t="s">
         <v>119</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
-      <c r="K16" s="96"/>
-      <c r="L16" s="98"/>
-      <c r="M16" s="98"/>
+      <c r="K16" s="104"/>
+      <c r="L16" s="97"/>
+      <c r="M16" s="97"/>
     </row>
     <row r="17" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="105"/>
-      <c r="B17" s="106"/>
-      <c r="C17" s="107"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="103"/>
       <c r="G17" s="13" t="s">
         <v>10</v>
       </c>
@@ -2926,45 +2920,45 @@
       <c r="J17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="97"/>
-      <c r="L17" s="99"/>
-      <c r="M17" s="99"/>
+      <c r="K17" s="105"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="98"/>
     </row>
     <row r="18" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="85"/>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
-      <c r="L18" s="86"/>
-      <c r="M18" s="87"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
+      <c r="L18" s="76"/>
+      <c r="M18" s="77"/>
     </row>
     <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="94" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="104"/>
+      <c r="B22" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A9:M9"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="A12:M12"/>
-    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A18:M18"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="K13:K14"/>
@@ -2981,15 +2975,15 @@
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="A13:C14"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A9:M9"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="A12:M12"/>
+    <mergeCell ref="D10:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="68" orientation="landscape" verticalDpi="300" r:id="rId1"/>
@@ -2997,7 +2991,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3018,51 +3012,51 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
     </row>
     <row r="4" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="K4" s="18">
         <f ca="1">TODAY()</f>
-        <v>43802</v>
+        <v>43843</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
@@ -3089,12 +3083,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="94" t="s">
+      <c r="B7" s="79"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="102" t="s">
         <v>119</v>
       </c>
       <c r="E7" s="14" t="s">
@@ -3115,56 +3109,56 @@
       <c r="J7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="100"/>
+      <c r="K7" s="96"/>
     </row>
     <row r="8" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="105"/>
-      <c r="B8" s="106"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="95"/>
+      <c r="A8" s="99"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="103"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="100"/>
+      <c r="K8" s="96"/>
     </row>
     <row r="9" spans="1:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="85"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="87"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="77"/>
     </row>
     <row r="10" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="94" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="102" t="s">
         <v>119</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="96"/>
-      <c r="J10" s="98"/>
-      <c r="K10" s="98"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
     </row>
     <row r="11" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="105"/>
-      <c r="B11" s="106"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="95"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="103"/>
       <c r="E11" s="13" t="s">
         <v>10</v>
       </c>
@@ -3177,31 +3171,31 @@
       <c r="H11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="97"/>
-      <c r="J11" s="99"/>
-      <c r="K11" s="99"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
     </row>
     <row r="12" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="85"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="87"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="77"/>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="94" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="104"/>
+      <c r="B18" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3226,7 +3220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3247,55 +3241,55 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
     </row>
     <row r="4" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="M4" s="18">
         <f ca="1">TODAY()</f>
-        <v>43802</v>
+        <v>43843</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:13" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
@@ -3328,18 +3322,18 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="94" t="s">
+      <c r="B7" s="79"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="94" t="s">
+      <c r="F7" s="102" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="14" t="s">
@@ -3360,68 +3354,68 @@
       <c r="L7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="100"/>
+      <c r="M7" s="96"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="105"/>
-      <c r="B8" s="106"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
+      <c r="A8" s="99"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
-      <c r="M8" s="100"/>
+      <c r="M8" s="96"/>
     </row>
     <row r="9" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="85"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="87"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="77"/>
     </row>
     <row r="10" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="94" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="94" t="s">
+      <c r="E10" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="94" t="s">
+      <c r="F10" s="102" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="98"/>
-      <c r="M10" s="98"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="97"/>
     </row>
     <row r="11" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="105"/>
-      <c r="B11" s="106"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="103"/>
       <c r="G11" s="13" t="s">
         <v>10</v>
       </c>
@@ -3434,41 +3428,41 @@
       <c r="J11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="97"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="99"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
     </row>
     <row r="12" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="85"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="87"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="77"/>
     </row>
     <row r="13" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="94" t="s">
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="94" t="s">
+      <c r="E13" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="94" t="s">
+      <c r="F13" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="101"/>
+      <c r="G13" s="106"/>
       <c r="H13" s="14" t="s">
         <v>8</v>
       </c>
@@ -3481,17 +3475,17 @@
       <c r="K13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L13" s="100"/>
-      <c r="M13" s="98"/>
+      <c r="L13" s="96"/>
+      <c r="M13" s="97"/>
     </row>
     <row r="14" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="105"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="95"/>
-      <c r="F14" s="95"/>
-      <c r="G14" s="102"/>
+      <c r="A14" s="99"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="107"/>
       <c r="H14" s="9" t="s">
         <v>10</v>
       </c>
@@ -3502,35 +3496,51 @@
       <c r="K14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="100"/>
-      <c r="M14" s="99"/>
+      <c r="L14" s="96"/>
+      <c r="M14" s="98"/>
     </row>
     <row r="15" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="85"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
-      <c r="L15" s="86"/>
-      <c r="M15" s="87"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="77"/>
     </row>
     <row r="18" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" s="103" t="s">
+      <c r="B19" s="94" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="104"/>
+      <c r="B20" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A9:M9"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="A12:M12"/>
     <mergeCell ref="B19:B20"/>
@@ -3541,22 +3551,6 @@
     <mergeCell ref="A15:M15"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A9:M9"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="78" orientation="landscape" verticalDpi="300" r:id="rId1"/>
@@ -3564,14 +3558,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3588,57 +3582,57 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
     </row>
     <row r="3" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
     </row>
     <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="N4" s="18">
         <f ca="1">TODAY()</f>
-        <v>43802</v>
+        <v>43843</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
@@ -3674,24 +3668,24 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="94" t="s">
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="94" t="s">
+      <c r="F7" s="102" t="s">
         <v>38</v>
       </c>
       <c r="G7" s="108" t="s">
         <v>103</v>
       </c>
-      <c r="H7" s="101"/>
+      <c r="H7" s="106"/>
       <c r="I7" s="14" t="s">
         <v>8</v>
       </c>
@@ -3704,18 +3698,18 @@
       <c r="L7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="96"/>
     </row>
     <row r="8" spans="1:14" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="80"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
+      <c r="A8" s="86"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
       <c r="G8" s="109"/>
-      <c r="H8" s="102"/>
+      <c r="H8" s="107"/>
       <c r="I8" s="9" t="s">
         <v>10</v>
       </c>
@@ -3724,38 +3718,38 @@
       </c>
       <c r="K8" s="74"/>
       <c r="L8" s="10"/>
-      <c r="M8" s="100"/>
-      <c r="N8" s="100"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="96"/>
     </row>
     <row r="9" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="85"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="87"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="77"/>
     </row>
     <row r="10" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="94" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="94" t="s">
+      <c r="E10" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="94" t="s">
+      <c r="F10" s="102" t="s">
         <v>40</v>
       </c>
       <c r="G10" s="108" t="s">
@@ -3766,16 +3760,16 @@
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
-      <c r="M10" s="100"/>
-      <c r="N10" s="100"/>
+      <c r="M10" s="96"/>
+      <c r="N10" s="96"/>
     </row>
     <row r="11" spans="1:14" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="105"/>
-      <c r="B11" s="106"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="103"/>
       <c r="G11" s="109"/>
       <c r="H11" s="11" t="s">
         <v>41</v>
@@ -3792,38 +3786,38 @@
       <c r="L11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="M11" s="100"/>
-      <c r="N11" s="100"/>
+      <c r="M11" s="96"/>
+      <c r="N11" s="96"/>
     </row>
     <row r="12" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="85"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="87"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="77"/>
     </row>
     <row r="13" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="94" t="s">
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="102" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="108" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="94" t="s">
+      <c r="F13" s="102" t="s">
         <v>43</v>
       </c>
       <c r="G13" s="108" t="s">
@@ -3835,23 +3829,23 @@
       <c r="I13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="100"/>
+      <c r="J13" s="96"/>
       <c r="K13" s="14" t="s">
         <v>14</v>
       </c>
       <c r="L13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="100"/>
-      <c r="N13" s="100"/>
+      <c r="M13" s="96"/>
+      <c r="N13" s="96"/>
     </row>
     <row r="14" spans="1:14" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="105"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="95"/>
+      <c r="A14" s="99"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="103"/>
       <c r="E14" s="109"/>
-      <c r="F14" s="95"/>
+      <c r="F14" s="103"/>
       <c r="G14" s="109"/>
       <c r="H14" s="9" t="s">
         <v>27</v>
@@ -3859,45 +3853,45 @@
       <c r="I14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="100"/>
+      <c r="J14" s="96"/>
       <c r="K14" s="9" t="s">
         <v>27</v>
       </c>
       <c r="L14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M14" s="100"/>
-      <c r="N14" s="100"/>
+      <c r="M14" s="96"/>
+      <c r="N14" s="96"/>
     </row>
     <row r="15" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="85"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
-      <c r="L15" s="86"/>
-      <c r="M15" s="86"/>
-      <c r="N15" s="87"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="76"/>
+      <c r="N15" s="77"/>
     </row>
     <row r="16" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="83"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="94" t="s">
+      <c r="B16" s="79"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="94" t="s">
+      <c r="E16" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="94" t="s">
+      <c r="F16" s="102" t="s">
         <v>43</v>
       </c>
       <c r="G16" s="108" t="s">
@@ -3915,19 +3909,19 @@
       <c r="K16" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="L16" s="96"/>
+      <c r="L16" s="104"/>
       <c r="M16" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="N16" s="98"/>
+      <c r="N16" s="97"/>
     </row>
     <row r="17" spans="1:14" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="105"/>
-      <c r="B17" s="106"/>
-      <c r="C17" s="107"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="103"/>
       <c r="G17" s="109"/>
       <c r="H17" s="13" t="s">
         <v>10</v>
@@ -3941,112 +3935,147 @@
       <c r="K17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L17" s="97"/>
+      <c r="L17" s="105"/>
       <c r="M17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="N17" s="99"/>
+      <c r="N17" s="98"/>
     </row>
     <row r="18" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="85"/>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
-      <c r="L18" s="86"/>
-      <c r="M18" s="86"/>
-      <c r="N18" s="87"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
+      <c r="L18" s="76"/>
+      <c r="M18" s="76"/>
+      <c r="N18" s="77"/>
     </row>
     <row r="19" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="83"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="94" t="s">
+      <c r="B19" s="79"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="112" t="s">
+      <c r="E19" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="112" t="s">
+      <c r="F19" s="110" t="s">
         <v>106</v>
       </c>
-      <c r="G19" s="113" t="s">
+      <c r="G19" s="111" t="s">
         <v>107</v>
       </c>
-      <c r="H19" s="112" t="s">
+      <c r="H19" s="110" t="s">
         <v>106</v>
       </c>
-      <c r="I19" s="112" t="s">
+      <c r="I19" s="110" t="s">
         <v>106</v>
       </c>
-      <c r="J19" s="112" t="s">
+      <c r="J19" s="110" t="s">
         <v>106</v>
       </c>
-      <c r="K19" s="112" t="s">
+      <c r="K19" s="110" t="s">
         <v>106</v>
       </c>
-      <c r="L19" s="112" t="s">
+      <c r="L19" s="110" t="s">
         <v>106</v>
       </c>
-      <c r="M19" s="114"/>
-      <c r="N19" s="111" t="s">
+      <c r="M19" s="112"/>
+      <c r="N19" s="113" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="105"/>
-      <c r="B20" s="106"/>
-      <c r="C20" s="107"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="112"/>
-      <c r="F20" s="112"/>
-      <c r="G20" s="113"/>
-      <c r="H20" s="112"/>
-      <c r="I20" s="112"/>
-      <c r="J20" s="112"/>
-      <c r="K20" s="112"/>
-      <c r="L20" s="112"/>
-      <c r="M20" s="114"/>
-      <c r="N20" s="111"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="100"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="110"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="110"/>
+      <c r="K20" s="110"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="112"/>
+      <c r="N20" s="113"/>
     </row>
     <row r="21" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="85"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="86"/>
-      <c r="K21" s="86"/>
-      <c r="L21" s="86"/>
-      <c r="M21" s="86"/>
-      <c r="N21" s="87"/>
+      <c r="A21" s="75"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="77"/>
     </row>
     <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C25" s="103" t="s">
+      <c r="C25" s="94" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="104"/>
+      <c r="C26" s="95"/>
     </row>
     <row r="27" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="H27" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="A12:N12"/>
+    <mergeCell ref="A13:C14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A15:N15"/>
+    <mergeCell ref="A16:C17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="A10:C11"/>
     <mergeCell ref="A9:N9"/>
     <mergeCell ref="A21:N21"/>
     <mergeCell ref="M13:M14"/>
@@ -4063,41 +4092,6 @@
     <mergeCell ref="K19:K20"/>
     <mergeCell ref="L19:L20"/>
     <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A15:N15"/>
-    <mergeCell ref="A16:C17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="A12:N12"/>
-    <mergeCell ref="A13:C14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="N13:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="60" orientation="landscape" verticalDpi="300" r:id="rId1"/>
@@ -4105,7 +4099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4129,55 +4123,55 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
     </row>
     <row r="4" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="M4" s="18">
         <f ca="1">TODAY()</f>
-        <v>43802</v>
+        <v>43843</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:13" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
@@ -4210,33 +4204,33 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="85"/>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
-      <c r="L7" s="86"/>
-      <c r="M7" s="87"/>
+      <c r="A7" s="75"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="77"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="84"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="108" t="s">
         <v>70</v>
       </c>
       <c r="E8" s="108" t="s">
         <v>117</v>
       </c>
-      <c r="F8" s="94" t="s">
+      <c r="F8" s="102" t="s">
         <v>119</v>
       </c>
       <c r="G8" s="14" t="s">
@@ -4257,68 +4251,68 @@
       <c r="L8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="100"/>
+      <c r="M8" s="96"/>
     </row>
     <row r="9" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="105"/>
-      <c r="B9" s="106"/>
-      <c r="C9" s="107"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="101"/>
       <c r="D9" s="109"/>
       <c r="E9" s="109"/>
-      <c r="F9" s="95"/>
+      <c r="F9" s="103"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="100"/>
+      <c r="M9" s="96"/>
     </row>
     <row r="10" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="85"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="87"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="77"/>
     </row>
     <row r="11" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="83"/>
-      <c r="C11" s="84"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="108" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="94" t="s">
+      <c r="E11" s="102" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="94" t="s">
+      <c r="F11" s="102" t="s">
         <v>119</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
-      <c r="K11" s="96"/>
-      <c r="L11" s="98"/>
-      <c r="M11" s="98"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="97"/>
+      <c r="M11" s="97"/>
     </row>
     <row r="12" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="105"/>
-      <c r="B12" s="106"/>
-      <c r="C12" s="107"/>
+      <c r="A12" s="99"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="101"/>
       <c r="D12" s="109"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
+      <c r="E12" s="103"/>
+      <c r="F12" s="103"/>
       <c r="G12" s="13" t="s">
         <v>10</v>
       </c>
@@ -4331,45 +4325,36 @@
       <c r="J12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="97"/>
-      <c r="L12" s="99"/>
-      <c r="M12" s="99"/>
+      <c r="K12" s="105"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
     </row>
     <row r="13" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="85"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="87"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="77"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="94" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="104"/>
+      <c r="B17" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:M7"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="M8:M9"/>
     <mergeCell ref="A13:M13"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A10:M10"/>
@@ -4380,6 +4365,15 @@
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="M11:M12"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:M7"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="M8:M9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="69" orientation="landscape" verticalDpi="300" r:id="rId1"/>
@@ -4387,7 +4381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4428,7 +4422,7 @@
       <c r="A3" s="1"/>
       <c r="G3" s="18">
         <f ca="1">TODAY()</f>
-        <v>43802</v>
+        <v>43843</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>